<commit_message>
improved after tutorial practical 8
</commit_message>
<xml_diff>
--- a/practical 8/autophagosome (myself).xlsx
+++ b/practical 8/autophagosome (myself).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -50,6 +50,9 @@
     <t>The lipid bilayer surrounding an autophagosome, a double-membrane-bounded vesicle in which endogenous cellular material is sequestered.</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>GO:0016236</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>The major inducible pathway for the general turnover of cytoplasmic constituents in eukaryotic cells, it is also responsible for the degradation of active cytoplasmic enzymes and organelles during nutrient starvation. Macroautophagy involves the formation of double-membrane-bounded autophagosomes which enclose the cytoplasmic constituent targeted for degradation in a membrane-bounded structure.  Autophagosomes then fuse with a lysosome (or vacuole) releasing single-membrane-bounded autophagic bodies that are then degraded within the lysosome (or vacuole). Some types of macroautophagy, e.g. pexophagy, mitophagy, involve selective targeting of the targets to be degraded.</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>GO:0016237</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
     <t>The transfer of cytosolic components into the lysosomal compartment by direct invagination of the lysosomal membrane without prior sequestration into an autophagosome. The engulfing membranes fuse, resulting in the lysosomal delivery of the cargo wrapped in a single membrane derived from the invaginated lysosomal membrane. In S. cerevisiae, the vacuole is the lysosomal compartment.</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>GO:0016240</t>
   </si>
   <si>
@@ -86,6 +95,9 @@
     <t>Any process that modulates the size of the autophagosome.</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>GO:0030399</t>
   </si>
   <si>
@@ -318,6 +330,9 @@
   </si>
   <si>
     <t>A process that is carried out at the cellular level which results in the assembly, arrangement of constituent parts, or disassembly of an autophagosome.</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>GO:1990316</t>
@@ -727,46 +742,46 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -774,27 +789,27 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -802,13 +817,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -816,13 +831,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -830,13 +845,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -844,13 +859,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -858,13 +873,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -872,13 +887,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -886,27 +901,27 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -914,13 +929,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -928,13 +943,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -942,13 +957,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -956,13 +971,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -970,13 +985,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -984,13 +999,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -998,13 +1013,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -1012,27 +1027,27 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1040,13 +1055,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -1054,13 +1069,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1068,27 +1083,27 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1096,13 +1111,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1110,13 +1125,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1124,13 +1139,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1138,27 +1153,27 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -1166,13 +1181,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -1180,16 +1195,16 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>